<commit_message>
update tests and prepare new release
</commit_message>
<xml_diff>
--- a/well_profile/tests/trajectory1.xlsx
+++ b/well_profile/tests/trajectory1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanc/PycharmProjects/well_profile/well_profile/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D401978D-ED87-7E4E-B3C5-30AA2907AEF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A27DF9-DE57-0D41-BC29-A4E67C563125}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,13 +35,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>md</t>
+    <t>MD (ft)</t>
   </si>
   <si>
-    <t>inclination</t>
+    <t>Incl</t>
   </si>
   <si>
-    <t>azimuth</t>
+    <t>Azi</t>
   </si>
 </sst>
 </file>
@@ -314,7 +314,7 @@
   <dimension ref="A1:W999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>